<commit_message>
Added Nescius O/F Graph
</commit_message>
<xml_diff>
--- a/1_DesignCode/ISP derivation method accuracy analysis.xlsx
+++ b/1_DesignCode/ISP derivation method accuracy analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\LADS-GIT-Repos\1_DesignCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0064CB62-BC30-44FA-9D61-511444D5FE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D8A850-22D3-4202-9990-7E59979A942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{F200D95B-9822-4F7C-A1C8-390616B6BA68}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="RPA raw" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -486,13 +485,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8916,16 +8915,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>5043</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>107016</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>173131</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>118222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>425823</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>593911</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9466,50 +9465,50 @@
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
-      <c r="T20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
@@ -12807,7 +12806,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12890,19 +12889,19 @@
       <c r="U1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="12" t="s">
         <v>93</v>
       </c>
     </row>
@@ -12973,7 +12972,7 @@
         <f>L2-B2</f>
         <v>34.1019367991845</v>
       </c>
-      <c r="V2" s="13"/>
+      <c r="V2" s="14"/>
       <c r="X2">
         <v>101325</v>
       </c>
@@ -13042,7 +13041,7 @@
         <f t="shared" ref="U3:U8" si="6">L3-B3</f>
         <v>158.26197757390418</v>
       </c>
-      <c r="V3" s="13"/>
+      <c r="V3" s="14"/>
       <c r="X3">
         <v>101325</v>
       </c>
@@ -13111,7 +13110,7 @@
         <f t="shared" si="6"/>
         <v>13.103975535168161</v>
       </c>
-      <c r="V4" s="13"/>
+      <c r="V4" s="14"/>
       <c r="X4">
         <v>101325</v>
       </c>
@@ -13180,7 +13179,7 @@
         <f t="shared" si="6"/>
         <v>12.093781855249745</v>
       </c>
-      <c r="V5" s="13"/>
+      <c r="V5" s="14"/>
       <c r="X5">
         <v>101325</v>
       </c>
@@ -13252,7 +13251,7 @@
         <f t="shared" si="6"/>
         <v>19.897737003058069</v>
       </c>
-      <c r="V6" s="13"/>
+      <c r="V6" s="14"/>
       <c r="X6">
         <v>101325</v>
       </c>
@@ -13324,7 +13323,7 @@
         <f t="shared" si="6"/>
         <v>43.293170234454635</v>
       </c>
-      <c r="V7" s="13"/>
+      <c r="V7" s="14"/>
       <c r="X7">
         <v>101325</v>
       </c>
@@ -13403,7 +13402,7 @@
         <f t="shared" si="6"/>
         <v>45.355555555555554</v>
       </c>
-      <c r="V8" s="13"/>
+      <c r="V8" s="14"/>
       <c r="X8">
         <v>101325</v>
       </c>
@@ -13468,10 +13467,10 @@
         <f t="shared" si="5"/>
         <v>22.048999999999978</v>
       </c>
-      <c r="V9" s="12" t="s">
+      <c r="V9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="W9" s="12"/>
+      <c r="W9" s="13"/>
       <c r="X9" t="s">
         <v>91</v>
       </c>
@@ -13601,10 +13600,10 @@
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="V12" s="12" t="s">
+      <c r="V12" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="W12" s="12"/>
+      <c r="W12" s="13"/>
       <c r="X12" t="s">
         <v>90</v>
       </c>
@@ -13677,12 +13676,12 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="7">
         <f>MEDIAN(P2:P9)</f>
         <v>0.11167318770628881</v>
@@ -13701,12 +13700,12 @@
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="7">
         <f>AVERAGE(P15:S15)</f>
         <v>0.10533781967142833</v>
@@ -14767,8 +14766,8 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added gitignore file and chamber graphics
</commit_message>
<xml_diff>
--- a/1_DesignCode/ISP derivation method accuracy analysis.xlsx
+++ b/1_DesignCode/ISP derivation method accuracy analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\LADS-GIT-Repos\1_DesignCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D8A850-22D3-4202-9990-7E59979A942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7383065-2D34-4788-949F-FBAA63A47030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{F200D95B-9822-4F7C-A1C8-390616B6BA68}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="6" xr2:uid="{F200D95B-9822-4F7C-A1C8-390616B6BA68}"/>
   </bookViews>
   <sheets>
     <sheet name="Alex Analysis" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Accuracy Analysis" sheetId="5" r:id="rId4"/>
     <sheet name="Analysis 2 raw" sheetId="3" r:id="rId5"/>
     <sheet name="CEArun Nescius" sheetId="6" r:id="rId6"/>
-    <sheet name="RPA raw" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="RPA raw" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
   <si>
     <t>O/F</t>
   </si>
@@ -384,6 +385,33 @@
   </si>
   <si>
     <t>Max ther</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Ye80</t>
+  </si>
+  <si>
+    <t>Yn80</t>
+  </si>
+  <si>
+    <t>Ye80A1</t>
+  </si>
+  <si>
+    <t>Ye80A2</t>
+  </si>
+  <si>
+    <t>Ye80B</t>
+  </si>
+  <si>
+    <t>Yn80A1</t>
+  </si>
+  <si>
+    <t>Yn80A2</t>
+  </si>
+  <si>
+    <t>Yn80B</t>
   </si>
 </sst>
 </file>
@@ -5965,6 +5993,557 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ye80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6678848332536515E-2"/>
+                  <c:y val="-1.4053246059468083E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-977D-4C2C-AE75-3D9A39EFE614}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yn80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2548260512937297E-2"/>
+                  <c:y val="-5.8689197412413872E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-977D-4C2C-AE75-3D9A39EFE614}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="66948960"/>
+        <c:axId val="66950400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="66948960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66950400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66950400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66948960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6126,6 +6705,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8745,6 +9364,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8915,16 +10050,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>173131</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>118222</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285190</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>593911</xdr:colOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8946,6 +10081,1991 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>169376</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>172484</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0668A76-AC05-57AB-01D1-9CBFBEEE5551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3697381" y="169376"/>
+          <a:ext cx="8443072" cy="6099108"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>275896</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>72259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>308741</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04047FFF-AEBF-991E-EB65-0A9CF77F620B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4552293" y="3120259"/>
+          <a:ext cx="1865586" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>302172</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>303486</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69F8DA89-B558-4BD0-A8BC-485CAAEE6FA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6411310" y="3128142"/>
+          <a:ext cx="1314" cy="2330668"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>264072</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1314</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296917</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7883</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DE3FC74-F66B-47C1-B2D7-9E371736531C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4540469" y="3811314"/>
+          <a:ext cx="1865586" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>505810</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>506452</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>116159</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0224715-7C72-492E-BF9F-EEE3707B2E97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6592517" y="2995448"/>
+          <a:ext cx="642" cy="2454711"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>275896</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>144517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>507124</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E269A541-9B86-4FA8-8468-F2109168F4F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4552293" y="3002017"/>
+          <a:ext cx="2063969" cy="7883"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>282305</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>84114</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>513533</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91997</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB737FE-3B49-4E08-B168-99807C287009}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4543000" y="3894114"/>
+          <a:ext cx="2057240" cy="7883"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>221263</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>223345</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>135866</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC7A05F-211B-45EB-B40D-9D65908DDC18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6941315" y="2883776"/>
+          <a:ext cx="2082" cy="2586090"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>275896</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>206266</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>39414</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64066A74-9887-4A05-AC5E-48CD82A0933D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4552293" y="2886404"/>
+          <a:ext cx="2374025" cy="10510"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283779</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>10511</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>214149</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>21021</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88BC6B1C-1659-48FB-892B-33F14CD1A2FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4560176" y="4011011"/>
+          <a:ext cx="2374025" cy="10510"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>478968</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490904</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121212</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1D0DA1-F7BA-4832-90B2-FE2F367F8B07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7168449" y="2769577"/>
+          <a:ext cx="11936" cy="2685635"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>278423</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>496817</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47EA1A10-102F-4FC3-AF9D-20EDCE858D42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4535365" y="2776500"/>
+          <a:ext cx="2650933" cy="7731"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>262304</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>480698</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>108439</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7254D3-0D60-4202-8D4C-F5B1D6608529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4519246" y="4101208"/>
+          <a:ext cx="2650933" cy="7731"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>119948</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>154342</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2A2F07A-D98F-461A-8CD9-B09E60F9B84D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7424057" y="2710543"/>
+          <a:ext cx="11091" cy="2777799"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283029</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>49629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>116444</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>59871</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDA23C7-6294-47A2-8B9E-A7E50CF62F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4550229" y="2716629"/>
+          <a:ext cx="2881415" cy="10242"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>277586</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>169372</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>111001</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D812B8F0-138A-44F8-A0DE-8BC466B7FA0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4544786" y="4169872"/>
+          <a:ext cx="2881415" cy="10242"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>310816</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>140368</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314389</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114928</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA519052-F31D-43E0-B8B6-55CB663ADAD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7650079" y="2616868"/>
+          <a:ext cx="3573" cy="2832060"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>280737</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>144879</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>307946</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>155408</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1148E31-3E55-4607-AB24-89B6503CE0A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4561974" y="2621379"/>
+          <a:ext cx="3085235" cy="10529"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>277729</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>26568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304938</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>37097</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD516B88-D46D-4AEE-8E3D-CBD37855DC12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4558966" y="4217568"/>
+          <a:ext cx="3085235" cy="10529"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>479534</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>65690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>480341</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>141203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6E25EB7-6C0D-4777-B9FF-358BC14F01CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7810500" y="2542190"/>
+          <a:ext cx="807" cy="2933013"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>269327</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>72621</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>470441</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>91966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0459AF6A-179E-4EC5-9600-715C9C41EBB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4530022" y="2549121"/>
+          <a:ext cx="3244468" cy="19345"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>259474</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>55246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>460588</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>74591</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{440FB184-E4BB-467D-A7AB-67FCAA30AA28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4526674" y="4246246"/>
+          <a:ext cx="3249114" cy="19345"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22788</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>141203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD2EE58E-732E-45BD-85EE-5B02DA8D34EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7947588" y="2514600"/>
+          <a:ext cx="4426" cy="2960603"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283029</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>34521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22438</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048DE7B8-B4AB-453A-9820-9DB5FAE17C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4550229" y="2511021"/>
+          <a:ext cx="3397009" cy="9022"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293914</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>110721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>33323</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AFA073E-285F-4152-AA92-7F75C0FDDAE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4561114" y="4301721"/>
+          <a:ext cx="3397009" cy="9022"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>437492</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>439615</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322F6BD9-674A-478C-BCAA-465B330A0E2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8951377" y="2227385"/>
+          <a:ext cx="2123" cy="3240491"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>129771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457658</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Connector 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{720D30F0-9A16-4007-9FE4-E7FD8FDCFCFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4542692" y="2225271"/>
+          <a:ext cx="4428851" cy="2114"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276958</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>77017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>448866</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>79131</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A51F2C6-B8B7-4754-AE27-CB13D0DE7F59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4533900" y="4458517"/>
+          <a:ext cx="4428851" cy="2114"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428572</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>434578</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>125593</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1392ECC6-39E0-41EA-B441-DE7A20C12862}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9536853" y="2083594"/>
+          <a:ext cx="6006" cy="3375999"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>292161</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>129771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>464069</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D226E8B5-09A8-4B42-A0F5-A975E4D8FCF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4542692" y="2225271"/>
+          <a:ext cx="4422440" cy="2114"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>279797</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>186921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>425970</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB1E142-8618-4DCE-8431-66A2A769031B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4530328" y="2091921"/>
+          <a:ext cx="5003923" cy="3579"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>289322</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>160727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>435495</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>164306</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686267B8-308F-407B-B912-72EB586B8AF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4539853" y="4542227"/>
+          <a:ext cx="5003923" cy="3579"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>256761</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>268613</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142159</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Connector 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7A99152-C718-4063-9D5D-CF48608B613A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10063370" y="1987826"/>
+          <a:ext cx="11852" cy="3488333"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>289034</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>70964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>261871</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>72259</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576F0B5B-2CD6-46FF-A07E-06DB419F7F7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4565431" y="1975964"/>
+          <a:ext cx="5471061" cy="1295"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>279181</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>252018</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>182163</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Straight Connector 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D89ACE-489E-499B-9626-F67CA8D9BFEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4536123" y="4562368"/>
+          <a:ext cx="5446049" cy="1295"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>579782</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>603230</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137189</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Straight Connector 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC689E6-066D-4A82-BC74-03D74B9B0A53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10386391" y="1913283"/>
+          <a:ext cx="23448" cy="3557906"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295603</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>585064</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>177381</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51155F61-8F85-4113-9912-874C140ADEB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4572000" y="1885293"/>
+          <a:ext cx="5787685" cy="6588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>278423</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>353130</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>120788</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Straight Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66BC995C-80A9-45DD-8447-34D319DAE358}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4535365" y="4674577"/>
+          <a:ext cx="6764188" cy="18211"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>284285</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>358992</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>170611</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Straight Connector 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15AFD6F4-8D86-4B9C-ACA1-7794073B5335}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4541227" y="1676400"/>
+          <a:ext cx="6764188" cy="18211"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>319366</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>302558</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="69" name="Chart 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95774E5-BF57-38DA-3196-5653DA1F900B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14765,9 +17885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5734E33E-62FC-4879-B1EA-CA5295C290FA}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16782,6 +19902,220 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C556590-DD5A-422F-B14B-A5D0D88CE436}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>3.5</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>24.5</v>
+      </c>
+      <c r="C6">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>25.2</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>26.1</v>
+      </c>
+      <c r="C9">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="B17">
+        <v>-0.90920000000000001</v>
+      </c>
+      <c r="C17">
+        <v>15.663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="B19">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="C19">
+        <v>20.888000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A4F017-176D-4B58-A404-F75FE29B8864}">
   <dimension ref="A1:O70"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated code and such, pushing for merge and reset.
</commit_message>
<xml_diff>
--- a/1_DesignCode/ISP derivation method accuracy analysis.xlsx
+++ b/1_DesignCode/ISP derivation method accuracy analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\LADS-GIT-Repos\1_DesignCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE267D8D-E768-4B0B-9755-545738A23797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC3525F-349D-4852-BB90-64557B721DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{F200D95B-9822-4F7C-A1C8-390616B6BA68}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{F200D95B-9822-4F7C-A1C8-390616B6BA68}"/>
   </bookViews>
   <sheets>
     <sheet name="Alex Analysis" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -681,14 +681,14 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6450,175 +6450,175 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="57"/>
                 <c:pt idx="0">
-                  <c:v>58.674821610601427</c:v>
+                  <c:v>173.29255861365951</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.353720693170231</c:v>
+                  <c:v>175.02548419979613</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.135575942915395</c:v>
+                  <c:v>178.6544342507645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>152.21202854230376</c:v>
+                  <c:v>183.28236493374106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156.92150866462794</c:v>
+                  <c:v>190.50968399592253</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160.83588175331295</c:v>
+                  <c:v>199.4189602446483</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>164.14882772680937</c:v>
+                  <c:v>207.67584097859324</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>167.01325178389399</c:v>
+                  <c:v>215.01529051987768</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>169.51070336391439</c:v>
+                  <c:v>221.48827726809378</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>173.29255861365951</c:v>
+                  <c:v>227.20693170234455</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175.02548419979613</c:v>
+                  <c:v>232.23241590214064</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>178.6544342507645</c:v>
+                  <c:v>236.61569826707438</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>183.28236493374106</c:v>
+                  <c:v>240.38735983690108</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>190.50968399592253</c:v>
+                  <c:v>243.58817533129456</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>199.4189602446483</c:v>
+                  <c:v>246.24872579001016</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>207.67584097859324</c:v>
+                  <c:v>248.38939857288477</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>215.01529051987768</c:v>
+                  <c:v>250.04077471967381</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>221.48827726809378</c:v>
+                  <c:v>251.24362895005095</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>227.20693170234455</c:v>
+                  <c:v>252.03873598369009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>232.23241590214064</c:v>
+                  <c:v>252.46687054026501</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>236.61569826707438</c:v>
+                  <c:v>252.59938837920487</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>240.38735983690108</c:v>
+                  <c:v>252.47706422018348</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>243.58817533129456</c:v>
+                  <c:v>252.16106014271148</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>246.24872579001016</c:v>
+                  <c:v>251.69215086646278</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>248.38939857288477</c:v>
+                  <c:v>251.11111111111111</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250.04077471967381</c:v>
+                  <c:v>250.43832823649339</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>251.24362895005095</c:v>
+                  <c:v>249.70438328236492</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>252.03873598369009</c:v>
+                  <c:v>248.92966360856269</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>252.46687054026501</c:v>
+                  <c:v>248.12436289500508</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>252.59938837920487</c:v>
+                  <c:v>247.28848114169216</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>252.47706422018348</c:v>
+                  <c:v>246.44240570846074</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>252.16106014271148</c:v>
+                  <c:v>245.58613659531088</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>251.69215086646278</c:v>
+                  <c:v>244.71967380224257</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>251.11111111111111</c:v>
+                  <c:v>243.85321100917429</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>250.43832823649339</c:v>
+                  <c:v>242.99694189602448</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>249.70438328236492</c:v>
+                  <c:v>242.14067278287462</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>248.92966360856269</c:v>
+                  <c:v>241.28440366972475</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>248.12436289500508</c:v>
+                  <c:v>240.43832823649333</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>247.28848114169216</c:v>
+                  <c:v>239.60244648318042</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>246.44240570846074</c:v>
+                  <c:v>238.7665647298675</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>245.58613659531088</c:v>
+                  <c:v>237.95107033639144</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>244.71967380224257</c:v>
+                  <c:v>237.13557594291541</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>243.85321100917429</c:v>
+                  <c:v>236.3302752293578</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>242.99694189602448</c:v>
+                  <c:v>235.53516819571863</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>242.14067278287462</c:v>
+                  <c:v>234.75025484199796</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>241.28440366972475</c:v>
+                  <c:v>233.97553516819573</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>240.43832823649333</c:v>
+                  <c:v>233.21100917431193</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>239.60244648318042</c:v>
+                  <c:v>232.44648318042815</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>238.7665647298675</c:v>
+                  <c:v>231.70234454638123</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>237.95107033639144</c:v>
+                  <c:v>230.95820591233434</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>237.13557594291541</c:v>
+                  <c:v>230.22426095820589</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>236.3302752293578</c:v>
+                  <c:v>229.50050968399592</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>235.53516819571863</c:v>
+                  <c:v>228.78695208970439</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>234.75025484199796</c:v>
+                  <c:v>228.08358817533127</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>233.97553516819573</c:v>
+                  <c:v>227.38022426095819</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>233.21100917431193</c:v>
+                  <c:v>226.68705402650357</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>232.44648318042815</c:v>
+                  <c:v>226.00407747196735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6663,175 +6663,175 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="57"/>
                 <c:pt idx="0">
-                  <c:v>346.01648334937568</c:v>
+                  <c:v>157.52835897177252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>292.52094782009135</c:v>
+                  <c:v>166.24276238378664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>251.30015618299058</c:v>
+                  <c:v>175.08846645637163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220.42373472320014</c:v>
+                  <c:v>183.84637900184407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>198.18348189801191</c:v>
+                  <c:v>192.34103100855242</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>183.0750755133754</c:v>
+                  <c:v>200.4355025174998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>173.78075569595239</c:v>
+                  <c:v>208.0267050013922</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>169.15295813547073</c:v>
+                  <c:v>215.04100832894568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>168.1988720721738</c:v>
+                  <c:v>221.43020039729873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>170.06589750413787</c:v>
+                  <c:v>227.1677675153702</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>174.02797608920719</c:v>
+                  <c:v>232.24548362099563</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>179.47277021635182</c:v>
+                  <c:v>236.67029641469554</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>185.88966472119046</c:v>
+                  <c:v>240.46149849290634</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>192.85856572049761</c:v>
+                  <c:v>243.64817156351455</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>200.03947104036797</c:v>
+                  <c:v>246.26689182654115</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>207.16278671298187</c:v>
+                  <c:v>248.35968460281526</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>214.02036401654277</c:v>
+                  <c:v>249.97221629347041</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>220.45723153331801</c:v>
+                  <c:v>251.15221175310955</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>226.3639967004774</c:v>
+                  <c:v>251.94808515948637</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>231.66989132853359</c:v>
+                  <c:v>252.40777246252742</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>236.3364355621261</c:v>
+                  <c:v>252.57775349555084</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>240.35169475794919</c:v>
+                  <c:v>252.50225183150997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>243.72510375459842</c:v>
+                  <c:v>252.22260046711062</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>246.48283300908861</c:v>
+                  <c:v>251.77676141764834</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>248.66367107486167</c:v>
+                  <c:v>251.19898730539012</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250.31539789591534</c:v>
+                  <c:v>250.51961302433506</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>251.49162339208215</c:v>
+                  <c:v>249.76496556425116</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>252.2490658099623</c:v>
+                  <c:v>248.95738007672799</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>252.64524431448172</c:v>
+                  <c:v>248.1153102662106</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>252.7365602956952</c:v>
+                  <c:v>247.25352118872217</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>252.57674186574059</c:v>
+                  <c:v>246.38335254122535</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>252.21562602063477</c:v>
+                  <c:v>245.51304052442163</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>251.69825294170641</c:v>
+                  <c:v>244.64808636179907</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>251.06424691149277</c:v>
+                  <c:v>243.79165955782662</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>250.34745831865166</c:v>
+                  <c:v>242.94502397807764</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>249.57584122708886</c:v>
+                  <c:v>242.10797483419879</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>248.7715409836137</c:v>
+                  <c:v>241.27927465645541</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>247.95116633905218</c:v>
+                  <c:v>240.45707633681377</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>247.12622055794509</c:v>
+                  <c:v>239.63932132530067</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>246.30366599097852</c:v>
+                  <c:v>238.82410106259658</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>245.48659658528504</c:v>
+                  <c:v>238.00996973149427</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>244.67499280753054</c:v>
+                  <c:v>237.19619641035206</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>243.86653345412651</c:v>
+                  <c:v>236.3829447111566</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>243.05743882379556</c:v>
+                  <c:v>235.57136798507986</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>242.24331972688833</c:v>
+                  <c:v>234.7636081784608</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>241.42000680633737</c:v>
+                  <c:v>233.96268642197606</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>240.58433464546124</c:v>
+                  <c:v>233.17227343581794</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>239.73485513629294</c:v>
+                  <c:v>232.39632783380057</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>238.87245458484631</c:v>
+                  <c:v>231.63859040921056</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>238.0008490261871</c:v>
+                  <c:v>230.90192248515768</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>237.12693222575854</c:v>
+                  <c:v>230.18747641235291</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>236.26095084075951</c:v>
+                  <c:v>229.49368629721516</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>235.4164812164463</c:v>
+                  <c:v>228.81506704291314</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>234.6101822929968</c:v>
+                  <c:v>228.14080978656443</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>233.86129909567626</c:v>
+                  <c:v>227.45316181489807</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>233.19089128634096</c:v>
+                  <c:v>226.7255790418626</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>232.62076124674877</c:v>
+                  <c:v>225.92063913027482</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15540,16 +15540,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22191,50 +22191,50 @@
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
@@ -25615,7 +25615,7 @@
       <c r="U1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="16" t="s">
         <v>85</v>
       </c>
       <c r="W1" s="12" t="s">
@@ -25698,7 +25698,7 @@
         <f>L2-B2</f>
         <v>34.1019367991845</v>
       </c>
-      <c r="V2" s="14"/>
+      <c r="V2" s="16"/>
       <c r="X2">
         <v>101325</v>
       </c>
@@ -25767,7 +25767,7 @@
         <f t="shared" ref="U3:U8" si="6">L3-B3</f>
         <v>158.26197757390418</v>
       </c>
-      <c r="V3" s="14"/>
+      <c r="V3" s="16"/>
       <c r="X3">
         <v>101325</v>
       </c>
@@ -25836,7 +25836,7 @@
         <f t="shared" si="6"/>
         <v>13.103975535168161</v>
       </c>
-      <c r="V4" s="14"/>
+      <c r="V4" s="16"/>
       <c r="X4">
         <v>101325</v>
       </c>
@@ -25905,7 +25905,7 @@
         <f t="shared" si="6"/>
         <v>12.093781855249745</v>
       </c>
-      <c r="V5" s="14"/>
+      <c r="V5" s="16"/>
       <c r="X5">
         <v>101325</v>
       </c>
@@ -25977,7 +25977,7 @@
         <f t="shared" si="6"/>
         <v>19.897737003058069</v>
       </c>
-      <c r="V6" s="14"/>
+      <c r="V6" s="16"/>
       <c r="X6">
         <v>101325</v>
       </c>
@@ -26049,7 +26049,7 @@
         <f t="shared" si="6"/>
         <v>43.293170234454635</v>
       </c>
-      <c r="V7" s="14"/>
+      <c r="V7" s="16"/>
       <c r="X7">
         <v>101325</v>
       </c>
@@ -26128,7 +26128,7 @@
         <f t="shared" si="6"/>
         <v>45.355555555555554</v>
       </c>
-      <c r="V8" s="14"/>
+      <c r="V8" s="16"/>
       <c r="X8">
         <v>101325</v>
       </c>
@@ -26193,10 +26193,10 @@
         <f t="shared" si="5"/>
         <v>22.048999999999978</v>
       </c>
-      <c r="V9" s="13" t="s">
+      <c r="V9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="W9" s="13"/>
+      <c r="W9" s="15"/>
       <c r="X9" t="s">
         <v>91</v>
       </c>
@@ -26326,10 +26326,10 @@
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="V12" s="13" t="s">
+      <c r="V12" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="W12" s="13"/>
+      <c r="W12" s="15"/>
       <c r="X12" t="s">
         <v>90</v>
       </c>
@@ -26402,12 +26402,12 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
       <c r="P15" s="7">
         <f>MEDIAN(P2:P9)</f>
         <v>0.11167318770628881</v>
@@ -26426,12 +26426,12 @@
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
       <c r="P16" s="7">
         <f>AVERAGE(P15:S15)</f>
         <v>0.10533781967142833</v>
@@ -27491,9 +27491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5734E33E-62FC-4879-B1EA-CA5295C290FA}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29511,8 +29511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE545128-23C9-408D-84C5-1EBC491AB886}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29539,12 +29539,12 @@
       <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" cm="1">
@@ -29552,53 +29552,53 @@
         <v>0.5</v>
       </c>
       <c r="B2">
-        <f>'CEArun Nescius'!D3</f>
-        <v>58.674821610601427</v>
-      </c>
-      <c r="C2" cm="1">
-        <f t="array" ref="C2:C58">'CEArun Nescius'!C12:C68</f>
+        <f>'CEArun Nescius'!D12</f>
+        <v>173.29255861365951</v>
+      </c>
+      <c r="C2">
+        <f>'CEArun Nescius'!C12</f>
         <v>1170</v>
       </c>
       <c r="D2">
         <f>A2^7*$H$2+A2^6*$I$2+A2^5*$J$2+A2^4*$K$2+$L$2*A2^3+$M$2*A2^2+$N$2*A2+$O$2</f>
-        <v>346.01648334937568</v>
-      </c>
-      <c r="E2" s="15">
+        <v>157.52835897177252</v>
+      </c>
+      <c r="E2" s="13">
         <f>ABS((D2-B2)/B2)</f>
-        <v>4.8971885018369967</v>
+        <v>9.0968704992300822E-2</v>
       </c>
       <c r="F2">
         <f>A2^7*$H$4+A2^6*$I$4+A2^5*$J$4+A2^4*$K$4+$L$4*A2^3+$M$4*A2^2+$N$4*A2+$O$4</f>
         <v>1392.1673135620476</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="13">
         <f>ABS((F2-C2)/C2)</f>
         <v>0.1898865927880749</v>
       </c>
       <c r="H2" cm="1">
         <f t="array" ref="H2:O2">LINEST(B9:B58, A9:A58^{1,2,3,4,5,6,7})</f>
-        <v>-6.4825973616704742</v>
+        <v>-3.0265801688132168</v>
       </c>
       <c r="I2">
-        <v>116.23319956053916</v>
+        <v>45.460043948091581</v>
       </c>
       <c r="J2">
-        <v>-870.36376165268632</v>
+        <v>-280.89149960359259</v>
       </c>
       <c r="K2">
-        <v>3512.4756791539589</v>
+        <v>910.48302601893351</v>
       </c>
       <c r="L2">
-        <v>-8188.8087775445001</v>
+        <v>-1617.8976348072938</v>
       </c>
       <c r="M2">
-        <v>10882.695931102933</v>
+        <v>1450.5814648672063</v>
       </c>
       <c r="N2">
-        <v>-7453.1378681786991</v>
+        <v>-441.53907189345574</v>
       </c>
       <c r="O2">
-        <v>2181.4161710093331</v>
+        <v>169.07573525991938</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -29606,59 +29606,61 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B3">
-        <f>'CEArun Nescius'!D4</f>
-        <v>63.353720693170231</v>
+        <f>'CEArun Nescius'!D13</f>
+        <v>175.02548419979613</v>
       </c>
       <c r="C3">
+        <f>'CEArun Nescius'!C13</f>
         <v>1209.6600000000001</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D58" si="0">A3^7*$H$2+A3^6*$I$2+A3^5*$J$2+A3^4*$K$2+$L$2*A3^3+$M$2*A3^2+$N$2*A3+$O$2</f>
-        <v>292.52094782009135</v>
-      </c>
-      <c r="E3" s="15">
+        <v>166.24276238378664</v>
+      </c>
+      <c r="E3" s="13">
         <f t="shared" ref="E3:E58" si="1">ABS((D3-B3)/B3)</f>
-        <v>3.617265483692834</v>
+        <v>5.0179674440916158E-2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F58" si="2">A3^7*$H$4+A3^6*$I$4+A3^5*$J$4+A3^4*$K$4+$L$4*A3^3+$M$4*A3^2+$N$4*A3+$O$4</f>
         <v>1346.5312393588938</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <f t="shared" ref="G3:G58" si="3">ABS((F3-C3)/C3)</f>
         <v>0.11314852054204794</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4">
         <v>0.60000000000000009</v>
       </c>
       <c r="B4">
-        <f>'CEArun Nescius'!D5</f>
-        <v>67.135575942915395</v>
+        <f>'CEArun Nescius'!D14</f>
+        <v>178.6544342507645</v>
       </c>
       <c r="C4">
+        <f>'CEArun Nescius'!C14</f>
         <v>1250.29</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>251.30015618299058</v>
-      </c>
-      <c r="E4" s="15">
+        <v>175.08846645637163</v>
+      </c>
+      <c r="E4" s="13">
         <f t="shared" si="1"/>
-        <v>2.7431742061268407</v>
+        <v>1.9960141539994279E-2</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
         <v>1361.2159065512133</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <f t="shared" si="3"/>
         <v>8.8720142167987667E-2</v>
       </c>
@@ -29693,25 +29695,26 @@
         <v>0.65000000000000013</v>
       </c>
       <c r="B5">
-        <f>'CEArun Nescius'!D6</f>
-        <v>152.21202854230376</v>
+        <f>'CEArun Nescius'!D15</f>
+        <v>183.28236493374106</v>
       </c>
       <c r="C5">
+        <f>'CEArun Nescius'!C15</f>
         <v>1312.22</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>220.42373472320014</v>
-      </c>
-      <c r="E5" s="15">
+        <v>183.84637900184407</v>
+      </c>
+      <c r="E5" s="13">
         <f t="shared" si="1"/>
-        <v>0.44813610878287813</v>
+        <v>3.0772958888156234E-3</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
         <v>1422.1957812393193</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <f t="shared" si="3"/>
         <v>8.3808950663241913E-2</v>
       </c>
@@ -29745,25 +29748,26 @@
         <v>0.70000000000000018</v>
       </c>
       <c r="B6">
-        <f>'CEArun Nescius'!D7</f>
-        <v>156.92150866462794</v>
+        <f>'CEArun Nescius'!D16</f>
+        <v>190.50968399592253</v>
       </c>
       <c r="C6">
+        <f>'CEArun Nescius'!C16</f>
         <v>1428.18</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>198.18348189801191</v>
-      </c>
-      <c r="E6" s="15">
+        <v>192.34103100855242</v>
+      </c>
+      <c r="E6" s="13">
         <f t="shared" si="1"/>
-        <v>0.26294657491197654</v>
+        <v>9.6128814778207658E-3</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
         <v>1517.5146015789833</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <f t="shared" si="3"/>
         <v>6.2551360177977008E-2</v>
       </c>
@@ -29773,25 +29777,26 @@
         <v>0.75000000000000022</v>
       </c>
       <c r="B7">
-        <f>'CEArun Nescius'!D8</f>
-        <v>160.83588175331295</v>
+        <f>'CEArun Nescius'!D17</f>
+        <v>199.4189602446483</v>
       </c>
       <c r="C7">
+        <f>'CEArun Nescius'!C17</f>
         <v>1389.99</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>183.0750755133754</v>
-      </c>
-      <c r="E7" s="15">
+        <v>200.4355025174998</v>
+      </c>
+      <c r="E7" s="13">
         <f t="shared" si="1"/>
-        <v>0.13827258891254443</v>
+        <v>5.0975206750872417E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
         <v>1637.0759225111651</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <f t="shared" si="3"/>
         <v>0.17776093533850251</v>
       </c>
@@ -29801,25 +29806,26 @@
         <v>0.80000000000000027</v>
       </c>
       <c r="B8">
-        <f>'CEArun Nescius'!D9</f>
-        <v>164.14882772680937</v>
+        <f>'CEArun Nescius'!D18</f>
+        <v>207.67584097859324</v>
       </c>
       <c r="C8">
+        <f>'CEArun Nescius'!C18</f>
         <v>1754.7</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>173.78075569595239</v>
-      </c>
-      <c r="E8" s="15">
+        <v>208.0267050013922</v>
+      </c>
+      <c r="E8" s="13">
         <f t="shared" si="1"/>
-        <v>5.8678018615967859E-2</v>
+        <v>1.6894792439296059E-3</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
         <v>1772.4471885755192</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <f t="shared" si="3"/>
         <v>1.0114087066461049E-2</v>
       </c>
@@ -29829,25 +29835,26 @@
         <v>0.85000000000000031</v>
       </c>
       <c r="B9">
-        <f>'CEArun Nescius'!D10</f>
-        <v>167.01325178389399</v>
+        <f>'CEArun Nescius'!D19</f>
+        <v>215.01529051987768</v>
       </c>
       <c r="C9">
+        <f>'CEArun Nescius'!C19</f>
         <v>1913.94</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>169.15295813547073</v>
-      </c>
-      <c r="E9" s="15">
+        <v>215.04100832894568</v>
+      </c>
+      <c r="E9" s="13">
         <f t="shared" si="1"/>
-        <v>1.2811596257914894E-2</v>
+        <v>1.1960921014415499E-4</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
         <v>1916.6769081585044</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <f t="shared" si="3"/>
         <v>1.4299863937763569E-3</v>
       </c>
@@ -29857,25 +29864,26 @@
         <v>0.90000000000000036</v>
       </c>
       <c r="B10">
-        <f>'CEArun Nescius'!D11</f>
-        <v>169.51070336391439</v>
+        <f>'CEArun Nescius'!D20</f>
+        <v>221.48827726809378</v>
       </c>
       <c r="C10">
+        <f>'CEArun Nescius'!C20</f>
         <v>2066.91</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>168.1988720721738</v>
-      </c>
-      <c r="E10" s="15">
+        <v>221.43020039729873</v>
+      </c>
+      <c r="E10" s="13">
         <f t="shared" si="1"/>
-        <v>7.7389289626406729E-3</v>
+        <v>2.6221193966284237E-4</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
         <v>2064.1245025272583</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <f t="shared" si="3"/>
         <v>1.347662681365688E-3</v>
       </c>
@@ -29885,25 +29893,26 @@
         <v>0.9500000000000004</v>
       </c>
       <c r="B11">
-        <f>'CEArun Nescius'!D12</f>
-        <v>173.29255861365951</v>
+        <f>'CEArun Nescius'!D21</f>
+        <v>227.20693170234455</v>
       </c>
       <c r="C11">
+        <f>'CEArun Nescius'!C21</f>
         <v>2213.33</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>170.06589750413787</v>
-      </c>
-      <c r="E11" s="15">
+        <v>227.1677675153702</v>
+      </c>
+      <c r="E11" s="13">
         <f t="shared" si="1"/>
-        <v>1.861973263788666E-2</v>
+        <v>1.7237232456294164E-4</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
         <v>2210.302403000147</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <f t="shared" si="3"/>
         <v>1.3678922708556356E-3</v>
       </c>
@@ -29913,25 +29922,26 @@
         <v>1.0000000000000004</v>
       </c>
       <c r="B12">
-        <f>'CEArun Nescius'!D13</f>
-        <v>175.02548419979613</v>
+        <f>'CEArun Nescius'!D22</f>
+        <v>232.23241590214064</v>
       </c>
       <c r="C12">
+        <f>'CEArun Nescius'!C22</f>
         <v>2352.75</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>174.02797608920719</v>
-      </c>
-      <c r="E12" s="15">
+        <v>232.24548362099563</v>
+      </c>
+      <c r="E12" s="13">
         <f t="shared" si="1"/>
-        <v>5.6992164035395976E-3</v>
+        <v>5.6270003497231281E-5</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
         <v>2351.7299696051632</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="13">
         <f t="shared" si="3"/>
         <v>4.3354814359230457E-4</v>
       </c>
@@ -29941,25 +29951,26 @@
         <v>1.0500000000000005</v>
       </c>
       <c r="B13">
-        <f>'CEArun Nescius'!D14</f>
-        <v>178.6544342507645</v>
+        <f>'CEArun Nescius'!D23</f>
+        <v>236.61569826707438</v>
       </c>
       <c r="C13">
+        <f>'CEArun Nescius'!C23</f>
         <v>2484.5300000000002</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>179.47277021635182</v>
-      </c>
-      <c r="E13" s="15">
+        <v>236.67029641469554</v>
+      </c>
+      <c r="E13" s="13">
         <f t="shared" si="1"/>
-        <v>4.5805522209355484E-3</v>
+        <v>2.3074609174720645E-4</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
         <v>2485.7988045767997</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="13">
         <f t="shared" si="3"/>
         <v>5.106819305057854E-4</v>
       </c>
@@ -29969,25 +29980,26 @@
         <v>1.1000000000000005</v>
       </c>
       <c r="B14">
-        <f>'CEArun Nescius'!D15</f>
-        <v>183.28236493374106</v>
+        <f>'CEArun Nescius'!D24</f>
+        <v>240.38735983690108</v>
       </c>
       <c r="C14">
+        <f>'CEArun Nescius'!C24</f>
         <v>2607.89</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>185.88966472119046</v>
-      </c>
-      <c r="E14" s="15">
+        <v>240.46149849290634</v>
+      </c>
+      <c r="E14" s="13">
         <f t="shared" si="1"/>
-        <v>1.4225590052768931E-2</v>
+        <v>3.0841328785158356E-4</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
         <v>2610.6490340429591</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="13">
         <f t="shared" si="3"/>
         <v>1.0579564486842732E-3</v>
       </c>
@@ -29997,25 +30009,26 @@
         <v>1.1500000000000006</v>
       </c>
       <c r="B15">
-        <f>'CEArun Nescius'!D16</f>
-        <v>190.50968399592253</v>
+        <f>'CEArun Nescius'!D25</f>
+        <v>243.58817533129456</v>
       </c>
       <c r="C15">
+        <f>'CEArun Nescius'!C25</f>
         <v>2722.03</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>192.85856572049761</v>
-      </c>
-      <c r="E15" s="15">
+        <v>243.64817156351455</v>
+      </c>
+      <c r="E15" s="13">
         <f t="shared" si="1"/>
-        <v>1.2329461029526208E-2</v>
+        <v>2.4630190746487878E-4</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
         <v>2725.0561312524151</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="13">
         <f t="shared" si="3"/>
         <v>1.1117185528502149E-3</v>
       </c>
@@ -30025,25 +30038,26 @@
         <v>1.2000000000000006</v>
       </c>
       <c r="B16">
-        <f>'CEArun Nescius'!D17</f>
-        <v>199.4189602446483</v>
+        <f>'CEArun Nescius'!D26</f>
+        <v>246.24872579001016</v>
       </c>
       <c r="C16">
+        <f>'CEArun Nescius'!C26</f>
         <v>2826.16</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>200.03947104036797</v>
-      </c>
-      <c r="E16" s="15">
+        <v>246.26689182654115</v>
+      </c>
+      <c r="E16" s="13">
         <f t="shared" si="1"/>
-        <v>3.1115937770331429E-3</v>
+        <v>7.3771088450182043E-5</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
         <v>2828.3278546941001</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="13">
         <f t="shared" si="3"/>
         <v>7.6706721986732613E-4</v>
       </c>
@@ -30053,25 +30067,26 @@
         <v>1.2500000000000007</v>
       </c>
       <c r="B17">
-        <f>'CEArun Nescius'!D18</f>
-        <v>207.67584097859324</v>
+        <f>'CEArun Nescius'!D27</f>
+        <v>248.38939857288477</v>
       </c>
       <c r="C17">
+        <f>'CEArun Nescius'!C27</f>
         <v>2919.63</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>207.16278671298187</v>
-      </c>
-      <c r="E17" s="15">
+        <v>248.35968460281526</v>
+      </c>
+      <c r="E17" s="13">
         <f t="shared" si="1"/>
-        <v>2.4704571470316461E-3</v>
+        <v>1.1962656313123372E-4</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
         <v>2920.2108744593061</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="13">
         <f t="shared" si="3"/>
         <v>1.9895481937983923E-4</v>
       </c>
@@ -30081,25 +30096,26 @@
         <v>1.3000000000000007</v>
       </c>
       <c r="B18">
-        <f>'CEArun Nescius'!D19</f>
-        <v>215.01529051987768</v>
+        <f>'CEArun Nescius'!D28</f>
+        <v>250.04077471967381</v>
       </c>
       <c r="C18">
+        <f>'CEArun Nescius'!C28</f>
         <v>3001.98</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>214.02036401654277</v>
-      </c>
-      <c r="E18" s="15">
+        <v>249.97221629347041</v>
+      </c>
+      <c r="E18" s="13">
         <f t="shared" si="1"/>
-        <v>4.627236048791286E-3</v>
+        <v>2.7418898489759498E-4</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
         <v>3000.8066601974351</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="13">
         <f t="shared" si="3"/>
         <v>3.9085530302163796E-4</v>
       </c>
@@ -30109,25 +30125,26 @@
         <v>1.3500000000000008</v>
       </c>
       <c r="B19">
-        <f>'CEArun Nescius'!D20</f>
-        <v>221.48827726809378</v>
+        <f>'CEArun Nescius'!D29</f>
+        <v>251.24362895005095</v>
       </c>
       <c r="C19">
+        <f>'CEArun Nescius'!C29</f>
         <v>3073.03</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>220.45723153331801</v>
-      </c>
-      <c r="E19" s="15">
+        <v>251.15221175310955</v>
+      </c>
+      <c r="E19" s="13">
         <f t="shared" si="1"/>
-        <v>4.6550803839057143E-3</v>
+        <v>3.6385876658216569E-4</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
         <v>3070.496204016541</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="13">
         <f t="shared" si="3"/>
         <v>8.2452692731902573E-4</v>
       </c>
@@ -30137,25 +30154,26 @@
         <v>1.4000000000000008</v>
       </c>
       <c r="B20">
-        <f>'CEArun Nescius'!D21</f>
-        <v>227.20693170234455</v>
+        <f>'CEArun Nescius'!D30</f>
+        <v>252.03873598369009</v>
       </c>
       <c r="C20">
+        <f>'CEArun Nescius'!C30</f>
         <v>3132.99</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>226.3639967004774</v>
-      </c>
-      <c r="E20" s="15">
+        <v>251.94808515948637</v>
+      </c>
+      <c r="E20" s="13">
         <f t="shared" si="1"/>
-        <v>3.7099880516473205E-3</v>
+        <v>3.596702064463087E-4</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
         <v>3129.8731516800835</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="13">
         <f t="shared" si="3"/>
         <v>9.9484783542757682E-4</v>
       </c>
@@ -30165,25 +30183,26 @@
         <v>1.4500000000000008</v>
       </c>
       <c r="B21">
-        <f>'CEArun Nescius'!D22</f>
-        <v>232.23241590214064</v>
+        <f>'CEArun Nescius'!D31</f>
+        <v>252.46687054026501</v>
       </c>
       <c r="C21">
+        <f>'CEArun Nescius'!C31</f>
         <v>3182.52</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>231.66989132853359</v>
-      </c>
-      <c r="E21" s="15">
+        <v>252.40777246252742</v>
+      </c>
+      <c r="E21" s="13">
         <f t="shared" si="1"/>
-        <v>2.4222482956216128E-3</v>
+        <v>2.3408250599819686E-4</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
         <v>3179.6849154499796</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="13">
         <f t="shared" si="3"/>
         <v>8.9083008119992429E-4</v>
       </c>
@@ -30193,25 +30212,26 @@
         <v>1.5000000000000009</v>
       </c>
       <c r="B22">
-        <f>'CEArun Nescius'!D23</f>
-        <v>236.61569826707438</v>
+        <f>'CEArun Nescius'!D32</f>
+        <v>252.59938837920487</v>
       </c>
       <c r="C22">
+        <f>'CEArun Nescius'!C32</f>
         <v>3222.64</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>236.3364355621261</v>
-      </c>
-      <c r="E22" s="15">
+        <v>252.57775349555084</v>
+      </c>
+      <c r="E22" s="13">
         <f t="shared" si="1"/>
-        <v>1.1802374356120241E-3</v>
+        <v>8.564899461099261E-5</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
         <v>3220.7813419278391</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="13">
         <f t="shared" si="3"/>
         <v>5.7675014030756733E-4</v>
       </c>
@@ -30221,25 +30241,26 @@
         <v>1.5500000000000009</v>
       </c>
       <c r="B23">
-        <f>'CEArun Nescius'!D24</f>
-        <v>240.38735983690108</v>
+        <f>'CEArun Nescius'!D33</f>
+        <v>252.47706422018348</v>
       </c>
       <c r="C23">
+        <f>'CEArun Nescius'!C33</f>
         <v>3254.61</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>240.35169475794919</v>
-      </c>
-      <c r="E23" s="15">
+        <v>252.50225183150997</v>
+      </c>
+      <c r="E23" s="13">
         <f t="shared" si="1"/>
-        <v>1.4836503456792371E-4</v>
+        <v>9.9761978000984352E-5</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
         <v>3254.0705082447384</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="13">
         <f t="shared" si="3"/>
         <v>1.6576233565978072E-4</v>
       </c>
@@ -30249,25 +30270,26 @@
         <v>1.600000000000001</v>
       </c>
       <c r="B24">
-        <f>'CEArun Nescius'!D25</f>
-        <v>243.58817533129456</v>
+        <f>'CEArun Nescius'!D34</f>
+        <v>252.16106014271148</v>
       </c>
       <c r="C24">
+        <f>'CEArun Nescius'!C34</f>
         <v>3279.7</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>243.72510375459842</v>
-      </c>
-      <c r="E24" s="15">
+        <v>252.22260046711062</v>
+      </c>
+      <c r="E24" s="13">
         <f t="shared" si="1"/>
-        <v>5.6213083052010276E-4</v>
+        <v>2.4405165636723456E-4</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
         <v>3280.4812199512089</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="13">
         <f t="shared" si="3"/>
         <v>2.3819860085041181E-4</v>
       </c>
@@ -30277,25 +30299,26 @@
         <v>1.650000000000001</v>
       </c>
       <c r="B25">
-        <f>'CEArun Nescius'!D26</f>
-        <v>246.24872579001016</v>
+        <f>'CEArun Nescius'!D35</f>
+        <v>251.69215086646278</v>
       </c>
       <c r="C25">
+        <f>'CEArun Nescius'!C35</f>
         <v>3299.12</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>246.48283300908861</v>
-      </c>
-      <c r="E25" s="15">
+        <v>251.77676141764834</v>
+      </c>
+      <c r="E25" s="13">
         <f t="shared" si="1"/>
-        <v>9.5069413385752552E-4</v>
+        <v>3.3616682480675918E-4</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
         <v>3300.9317839575524</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="13">
         <f t="shared" si="3"/>
         <v>5.491718875192496E-4</v>
       </c>
@@ -30305,25 +30328,26 @@
         <v>1.7000000000000011</v>
       </c>
       <c r="B26">
-        <f>'CEArun Nescius'!D27</f>
-        <v>248.38939857288477</v>
+        <f>'CEArun Nescius'!D36</f>
+        <v>251.11111111111111</v>
       </c>
       <c r="C26">
+        <f>'CEArun Nescius'!C36</f>
         <v>3313.91</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>248.66367107486167</v>
-      </c>
-      <c r="E26" s="15">
+        <v>251.19898730539012</v>
+      </c>
+      <c r="E26" s="13">
         <f t="shared" si="1"/>
-        <v>1.1042037363620243E-3</v>
+        <v>3.4994944624382499E-4</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
         <v>3316.3046298769623</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="13">
         <f t="shared" si="3"/>
         <v>7.2259955067048489E-4</v>
       </c>
@@ -30333,25 +30357,26 @@
         <v>1.7500000000000011</v>
       </c>
       <c r="B27">
-        <f>'CEArun Nescius'!D28</f>
-        <v>250.04077471967381</v>
+        <f>'CEArun Nescius'!D37</f>
+        <v>250.43832823649339</v>
       </c>
       <c r="C27">
+        <f>'CEArun Nescius'!C37</f>
         <v>3324.94</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>250.31539789591534</v>
-      </c>
-      <c r="E27" s="15">
+        <v>250.51961302433506</v>
+      </c>
+      <c r="E27" s="13">
         <f t="shared" si="1"/>
-        <v>1.0983135712542063E-3</v>
+        <v>3.2457007844625491E-4</v>
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
         <v>3327.4263531202014</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="13">
         <f t="shared" si="3"/>
         <v>7.4778886843110827E-4</v>
       </c>
@@ -30361,25 +30386,26 @@
         <v>1.8000000000000012</v>
       </c>
       <c r="B28">
-        <f>'CEArun Nescius'!D29</f>
-        <v>251.24362895005095</v>
+        <f>'CEArun Nescius'!D38</f>
+        <v>249.70438328236492</v>
       </c>
       <c r="C28">
+        <f>'CEArun Nescius'!C38</f>
         <v>3332.9</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>251.49162339208215</v>
-      </c>
-      <c r="E28" s="15">
+        <v>249.76496556425116</v>
+      </c>
+      <c r="E28" s="13">
         <f t="shared" si="1"/>
-        <v>9.8706758482820095E-4</v>
+        <v>2.4261601294252996E-4</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
         <v>3335.0527530954278</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="13">
         <f t="shared" si="3"/>
         <v>6.4590989691489984E-4</v>
       </c>
@@ -30389,25 +30415,26 @@
         <v>1.8500000000000012</v>
       </c>
       <c r="B29">
-        <f>'CEArun Nescius'!D30</f>
-        <v>252.03873598369009</v>
+        <f>'CEArun Nescius'!D39</f>
+        <v>248.92966360856269</v>
       </c>
       <c r="C29">
+        <f>'CEArun Nescius'!C39</f>
         <v>3338.35</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>252.2490658099623</v>
-      </c>
-      <c r="E29" s="15">
+        <v>248.95738007672799</v>
+      </c>
+      <c r="E29" s="13">
         <f t="shared" si="1"/>
-        <v>8.3451389109420748E-4</v>
+        <v>1.1134256867385023E-4</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
         <v>3339.8584398619423</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="13">
         <f t="shared" si="3"/>
         <v>4.5185192144095329E-4</v>
       </c>
@@ -30417,25 +30444,26 @@
         <v>1.9000000000000012</v>
       </c>
       <c r="B30">
-        <f>'CEArun Nescius'!D31</f>
-        <v>252.46687054026501</v>
+        <f>'CEArun Nescius'!D40</f>
+        <v>248.12436289500508</v>
       </c>
       <c r="C30">
+        <f>'CEArun Nescius'!C40</f>
         <v>3341.74</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>252.64524431448172</v>
-      </c>
-      <c r="E30" s="15">
+        <v>248.1153102662106</v>
+      </c>
+      <c r="E30" s="13">
         <f t="shared" si="1"/>
-        <v>7.0652348894331826E-4</v>
+        <v>3.6484239954739887E-5</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
         <v>3342.4305825907213</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="13">
         <f t="shared" si="3"/>
         <v>2.0665359684521629E-4</v>
       </c>
@@ -30445,25 +30473,26 @@
         <v>1.9500000000000013</v>
       </c>
       <c r="B31">
-        <f>'CEArun Nescius'!D32</f>
-        <v>252.59938837920487</v>
+        <f>'CEArun Nescius'!D41</f>
+        <v>247.28848114169216</v>
       </c>
       <c r="C31">
+        <f>'CEArun Nescius'!C41</f>
         <v>3343.42</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>252.7365602956952</v>
-      </c>
-      <c r="E31" s="15">
+        <v>247.25352118872217</v>
+      </c>
+      <c r="E31" s="13">
         <f t="shared" si="1"/>
-        <v>5.4304136431402271E-4</v>
+        <v>1.4137315579189059E-4</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
         <v>3343.2663731806824</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="13">
         <f t="shared" si="3"/>
         <v>4.5949004108861915E-5</v>
       </c>
@@ -30473,25 +30502,26 @@
         <v>2.0000000000000013</v>
       </c>
       <c r="B32">
-        <f>'CEArun Nescius'!D33</f>
-        <v>252.47706422018348</v>
+        <f>'CEArun Nescius'!D42</f>
+        <v>246.44240570846074</v>
       </c>
       <c r="C32">
+        <f>'CEArun Nescius'!C42</f>
         <v>3343.69</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>252.57674186574059</v>
-      </c>
-      <c r="E32" s="15">
+        <v>246.38335254122535</v>
+      </c>
+      <c r="E32" s="13">
         <f t="shared" si="1"/>
-        <v>3.9479881416151064E-4</v>
+        <v>2.3962258875710634E-4</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
         <v>3342.7737783845078</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="13">
         <f t="shared" si="3"/>
         <v>2.7401511967087392E-4</v>
       </c>
@@ -30501,25 +30531,26 @@
         <v>2.0500000000000012</v>
       </c>
       <c r="B33">
-        <f>'CEArun Nescius'!D34</f>
-        <v>252.16106014271148</v>
+        <f>'CEArun Nescius'!D43</f>
+        <v>245.58613659531088</v>
       </c>
       <c r="C33">
+        <f>'CEArun Nescius'!C43</f>
         <v>3342.76</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>252.21562602063477</v>
-      </c>
-      <c r="E33" s="15">
+        <v>245.51304052442163</v>
+      </c>
+      <c r="E33" s="13">
         <f t="shared" si="1"/>
-        <v>2.1639295889862371E-4</v>
+        <v>2.9763923934232898E-4</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
         <v>3341.2751537921285</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="13">
         <f t="shared" si="3"/>
         <v>4.4419767134693162E-4</v>
       </c>
@@ -30529,25 +30560,26 @@
         <v>2.100000000000001</v>
       </c>
       <c r="B34">
-        <f>'CEArun Nescius'!D35</f>
-        <v>251.69215086646278</v>
+        <f>'CEArun Nescius'!D44</f>
+        <v>244.71967380224257</v>
       </c>
       <c r="C34">
+        <f>'CEArun Nescius'!C44</f>
         <v>3340.82</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>251.69825294170641</v>
-      </c>
-      <c r="E34" s="15">
+        <v>244.64808636179907</v>
+      </c>
+      <c r="E34" s="13">
         <f t="shared" si="1"/>
-        <v>2.4244201587635311E-5</v>
+        <v>2.9252834204635236E-4</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
         <v>3339.0132930238178</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="13">
         <f t="shared" si="3"/>
         <v>5.4079746175559901E-4</v>
       </c>
@@ -30557,25 +30589,26 @@
         <v>2.1500000000000008</v>
       </c>
       <c r="B35">
-        <f>'CEArun Nescius'!D36</f>
-        <v>251.11111111111111</v>
+        <f>'CEArun Nescius'!D45</f>
+        <v>243.85321100917429</v>
       </c>
       <c r="C35">
+        <f>'CEArun Nescius'!C45</f>
         <v>3338.02</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>251.06424691149277</v>
-      </c>
-      <c r="E35" s="15">
+        <v>243.79165955782662</v>
+      </c>
+      <c r="E35" s="13">
         <f t="shared" si="1"/>
-        <v>1.8662734361286144E-4</v>
+        <v>2.5241189604574272E-4</v>
       </c>
       <c r="F35">
         <f t="shared" si="2"/>
         <v>3336.1594854866562</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="13">
         <f t="shared" si="3"/>
         <v>5.5737069081185473E-4</v>
       </c>
@@ -30585,25 +30618,26 @@
         <v>2.2000000000000006</v>
       </c>
       <c r="B36">
-        <f>'CEArun Nescius'!D37</f>
-        <v>250.43832823649339</v>
+        <f>'CEArun Nescius'!D46</f>
+        <v>242.99694189602448</v>
       </c>
       <c r="C36">
+        <f>'CEArun Nescius'!C46</f>
         <v>3334.48</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>250.34745831865166</v>
-      </c>
-      <c r="E36" s="15">
+        <v>242.94502397807764</v>
+      </c>
+      <c r="E36" s="13">
         <f t="shared" si="1"/>
-        <v>3.6284349317297507E-4</v>
+        <v>2.1365667214467724E-4</v>
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
         <v>3332.8231560391432</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="13">
         <f t="shared" si="3"/>
         <v>4.9688226075934004E-4</v>
       </c>
@@ -30613,25 +30647,26 @@
         <v>2.2500000000000004</v>
       </c>
       <c r="B37">
-        <f>'CEArun Nescius'!D38</f>
-        <v>249.70438328236492</v>
+        <f>'CEArun Nescius'!D47</f>
+        <v>242.14067278287462</v>
       </c>
       <c r="C37">
+        <f>'CEArun Nescius'!C47</f>
         <v>3330.31</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>249.57584122708886</v>
-      </c>
-      <c r="E37" s="15">
+        <v>242.10797483419879</v>
+      </c>
+      <c r="E37" s="13">
         <f t="shared" si="1"/>
-        <v>5.1477692776703105E-4</v>
+        <v>1.3503699440511519E-4</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
         <v>3329.0626599227253</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G37" s="13">
         <f t="shared" si="3"/>
         <v>3.7454173253380536E-4</v>
       </c>
@@ -30641,25 +30676,26 @@
         <v>2.3000000000000003</v>
       </c>
       <c r="B38">
-        <f>'CEArun Nescius'!D39</f>
-        <v>248.92966360856269</v>
+        <f>'CEArun Nescius'!D48</f>
+        <v>241.28440366972475</v>
       </c>
       <c r="C38">
+        <f>'CEArun Nescius'!C48</f>
         <v>3325.58</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>248.7715409836137</v>
-      </c>
-      <c r="E38" s="15">
+        <v>241.27927465645541</v>
+      </c>
+      <c r="E38" s="13">
         <f t="shared" si="1"/>
-        <v>6.3521005354200068E-4</v>
+        <v>2.1257127237947253E-5</v>
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
         <v>3324.8968063046195</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="13">
         <f t="shared" si="3"/>
         <v>2.0543595263995939E-4</v>
       </c>
@@ -30669,25 +30705,26 @@
         <v>2.35</v>
       </c>
       <c r="B39">
-        <f>'CEArun Nescius'!D40</f>
-        <v>248.12436289500508</v>
+        <f>'CEArun Nescius'!D49</f>
+        <v>240.43832823649333</v>
       </c>
       <c r="C39">
+        <f>'CEArun Nescius'!C49</f>
         <v>3320.38</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>247.95116633905218</v>
-      </c>
-      <c r="E39" s="15">
+        <v>240.45707633681377</v>
+      </c>
+      <c r="E39" s="13">
         <f t="shared" si="1"/>
-        <v>6.9802317649149035E-4</v>
+        <v>7.7974674245764766E-5</v>
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
         <v>3320.3166837860917</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="13">
         <f t="shared" si="3"/>
         <v>1.9068966175065857E-5</v>
       </c>
@@ -30697,25 +30734,26 @@
         <v>2.4</v>
       </c>
       <c r="B40">
-        <f>'CEArun Nescius'!D41</f>
-        <v>247.28848114169216</v>
+        <f>'CEArun Nescius'!D50</f>
+        <v>239.60244648318042</v>
       </c>
       <c r="C40">
+        <f>'CEArun Nescius'!C50</f>
         <v>3314.75</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>247.12622055794509</v>
-      </c>
-      <c r="E40" s="15">
+        <v>239.63932132530067</v>
+      </c>
+      <c r="E40" s="13">
         <f t="shared" si="1"/>
-        <v>6.5615908593048247E-4</v>
+        <v>1.5390010687075316E-4</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
         <v>3315.2973612280184</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="13">
         <f t="shared" si="3"/>
         <v>1.65128962370742E-4</v>
       </c>
@@ -30725,25 +30763,26 @@
         <v>2.4499999999999997</v>
       </c>
       <c r="B41">
-        <f>'CEArun Nescius'!D42</f>
-        <v>246.44240570846074</v>
+        <f>'CEArun Nescius'!D51</f>
+        <v>238.7665647298675</v>
       </c>
       <c r="C41">
+        <f>'CEArun Nescius'!C51</f>
         <v>3308.75</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>246.30366599097852</v>
-      </c>
-      <c r="E41" s="15">
+        <v>238.82410106259658</v>
+      </c>
+      <c r="E41" s="13">
         <f t="shared" si="1"/>
-        <v>5.6297014746054669E-4</v>
+        <v>2.409731563302448E-4</v>
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
         <v>3309.8090372428996</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="13">
         <f t="shared" si="3"/>
         <v>3.2007170166970878E-4</v>
       </c>
@@ -30753,25 +30792,26 @@
         <v>2.4999999999999996</v>
       </c>
       <c r="B42">
-        <f>'CEArun Nescius'!D43</f>
-        <v>245.58613659531088</v>
+        <f>'CEArun Nescius'!D52</f>
+        <v>237.95107033639144</v>
       </c>
       <c r="C42">
+        <f>'CEArun Nescius'!C52</f>
         <v>3302.41</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>245.48659658528504</v>
-      </c>
-      <c r="E42" s="15">
+        <v>238.00996973149427</v>
+      </c>
+      <c r="E42" s="13">
         <f t="shared" si="1"/>
-        <v>4.0531607934311326E-4</v>
+        <v>2.47527338370704E-4</v>
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
         <v>3303.827211703232</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="13">
         <f t="shared" si="3"/>
         <v>4.2914468622374857E-4</v>
       </c>
@@ -30781,25 +30821,26 @@
         <v>2.5499999999999994</v>
       </c>
       <c r="B43">
-        <f>'CEArun Nescius'!D44</f>
-        <v>244.71967380224257</v>
+        <f>'CEArun Nescius'!D53</f>
+        <v>237.13557594291541</v>
       </c>
       <c r="C43">
+        <f>'CEArun Nescius'!C53</f>
         <v>3295.79</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>244.67499280753054</v>
-      </c>
-      <c r="E43" s="15">
+        <v>237.19619641035206</v>
+      </c>
+      <c r="E43" s="13">
         <f t="shared" si="1"/>
-        <v>1.8258031329402216E-4</v>
+        <v>2.5563632616323417E-4</v>
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
         <v>3297.3414526209235</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="13">
         <f t="shared" si="3"/>
         <v>4.707377050490339E-4</v>
       </c>
@@ -30809,25 +30850,26 @@
         <v>2.5999999999999992</v>
       </c>
       <c r="B44">
-        <f>'CEArun Nescius'!D45</f>
-        <v>243.85321100917429</v>
+        <f>'CEArun Nescius'!D54</f>
+        <v>236.3302752293578</v>
       </c>
       <c r="C44">
+        <f>'CEArun Nescius'!C54</f>
         <v>3288.9</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>243.86653345412651</v>
-      </c>
-      <c r="E44" s="15">
+        <v>236.3829447111566</v>
+      </c>
+      <c r="E44" s="13">
         <f t="shared" si="1"/>
-        <v>5.4633051158477069E-5</v>
+        <v>2.2286387872940118E-4</v>
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
         <v>3290.3623317467864</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="13">
         <f t="shared" si="3"/>
         <v>4.4462639386611821E-4</v>
       </c>
@@ -30837,25 +30879,26 @@
         <v>2.649999999999999</v>
       </c>
       <c r="B45">
-        <f>'CEArun Nescius'!D46</f>
-        <v>242.99694189602448</v>
+        <f>'CEArun Nescius'!D55</f>
+        <v>235.53516819571863</v>
       </c>
       <c r="C45">
+        <f>'CEArun Nescius'!C55</f>
         <v>3281.78</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>243.05743882379556</v>
-      </c>
-      <c r="E45" s="15">
+        <v>235.57136798507986</v>
+      </c>
+      <c r="E45" s="13">
         <f t="shared" si="1"/>
-        <v>2.4896168362879866E-4</v>
+        <v>1.5369165309171031E-4</v>
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
         <v>3282.9261022403516</v>
       </c>
-      <c r="G45" s="15">
+      <c r="G45" s="13">
         <f t="shared" si="3"/>
         <v>3.4923189255568949E-4</v>
       </c>
@@ -30865,25 +30908,26 @@
         <v>2.6999999999999988</v>
       </c>
       <c r="B46">
-        <f>'CEArun Nescius'!D47</f>
-        <v>242.14067278287462</v>
+        <f>'CEArun Nescius'!D56</f>
+        <v>234.75025484199796</v>
       </c>
       <c r="C46">
+        <f>'CEArun Nescius'!C56</f>
         <v>3274.45</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>242.24331972688833</v>
-      </c>
-      <c r="E46" s="15">
+        <v>234.7636081784608</v>
+      </c>
+      <c r="E46" s="13">
         <f t="shared" si="1"/>
-        <v>4.2391450735645736E-4</v>
+        <v>5.6883160667193461E-5</v>
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
         <v>3275.0966917604237</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="13">
         <f t="shared" si="3"/>
         <v>1.9749630027146285E-4</v>
       </c>
@@ -30893,25 +30937,26 @@
         <v>2.7499999999999987</v>
       </c>
       <c r="B47">
-        <f>'CEArun Nescius'!D48</f>
-        <v>241.28440366972475</v>
+        <f>'CEArun Nescius'!D57</f>
+        <v>233.97553516819573</v>
       </c>
       <c r="C47">
+        <f>'CEArun Nescius'!C57</f>
         <v>3266.93</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>241.42000680633737</v>
-      </c>
-      <c r="E47" s="15">
+        <v>233.96268642197606</v>
+      </c>
+      <c r="E47" s="13">
         <f t="shared" si="1"/>
-        <v>5.6200539508650753E-4</v>
+        <v>5.4914913264064182E-5</v>
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
         <v>3266.964584331392</v>
       </c>
-      <c r="G47" s="15">
+      <c r="G47" s="13">
         <f t="shared" si="3"/>
         <v>1.0586186845792541E-5</v>
       </c>
@@ -30921,25 +30966,26 @@
         <v>2.7999999999999985</v>
       </c>
       <c r="B48">
-        <f>'CEArun Nescius'!D49</f>
-        <v>240.43832823649333</v>
+        <f>'CEArun Nescius'!D58</f>
+        <v>233.21100917431193</v>
       </c>
       <c r="C48">
+        <f>'CEArun Nescius'!C58</f>
         <v>3259.23</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>240.58433464546124</v>
-      </c>
-      <c r="E48" s="15">
+        <v>233.17227343581794</v>
+      </c>
+      <c r="E48" s="13">
         <f t="shared" si="1"/>
-        <v>6.0725097383099299E-4</v>
+        <v>1.6609738378615954E-4</v>
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
         <v>3258.642164332181</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G48" s="13">
         <f t="shared" si="3"/>
         <v>1.8036028995162531E-4</v>
       </c>
@@ -30949,25 +30995,26 @@
         <v>2.8499999999999983</v>
       </c>
       <c r="B49">
-        <f>'CEArun Nescius'!D50</f>
-        <v>239.60244648318042</v>
+        <f>'CEArun Nescius'!D59</f>
+        <v>232.44648318042815</v>
       </c>
       <c r="C49">
+        <f>'CEArun Nescius'!C59</f>
         <v>3251.37</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>239.73485513629294</v>
-      </c>
-      <c r="E49" s="15">
+        <v>232.39632783380057</v>
+      </c>
+      <c r="E49" s="13">
         <f t="shared" si="1"/>
-        <v>5.5261811828709849E-4</v>
+        <v>2.1577158725453948E-4</v>
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
         <v>3250.2550959597866</v>
       </c>
-      <c r="G49" s="15">
+      <c r="G49" s="13">
         <f t="shared" si="3"/>
         <v>3.4290285024876665E-4</v>
       </c>
@@ -30977,25 +31024,26 @@
         <v>2.8999999999999981</v>
       </c>
       <c r="B50">
-        <f>'CEArun Nescius'!D51</f>
-        <v>238.7665647298675</v>
+        <f>'CEArun Nescius'!D60</f>
+        <v>231.70234454638123</v>
       </c>
       <c r="C50">
+        <f>'CEArun Nescius'!C60</f>
         <v>3243.37</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>238.87245458484631</v>
-      </c>
-      <c r="E50" s="15">
+        <v>231.63859040921056</v>
+      </c>
+      <c r="E50" s="13">
         <f t="shared" si="1"/>
-        <v>4.4348694759089398E-4</v>
+        <v>2.7515533904275949E-4</v>
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
         <v>3241.9293115217879</v>
       </c>
-      <c r="G50" s="15">
+      <c r="G50" s="13">
         <f t="shared" si="3"/>
         <v>4.4419492016390235E-4</v>
       </c>
@@ -31005,25 +31053,26 @@
         <v>2.949999999999998</v>
       </c>
       <c r="B51">
-        <f>'CEArun Nescius'!D52</f>
-        <v>237.95107033639144</v>
+        <f>'CEArun Nescius'!D61</f>
+        <v>230.95820591233434</v>
       </c>
       <c r="C51">
+        <f>'CEArun Nescius'!C61</f>
         <v>3235.24</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>238.0008490261871</v>
-      </c>
-      <c r="E51" s="15">
+        <v>230.90192248515768</v>
+      </c>
+      <c r="E51" s="13">
         <f t="shared" si="1"/>
-        <v>2.0919716698599656E-4</v>
+        <v>2.436952909047779E-4</v>
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
         <v>3233.7731819003093</v>
       </c>
-      <c r="G51" s="15">
+      <c r="G51" s="13">
         <f t="shared" si="3"/>
         <v>4.5338772384444416E-4</v>
       </c>
@@ -31033,25 +31082,26 @@
         <v>2.9999999999999978</v>
       </c>
       <c r="B52">
-        <f>'CEArun Nescius'!D53</f>
-        <v>237.13557594291541</v>
+        <f>'CEArun Nescius'!D62</f>
+        <v>230.22426095820589</v>
       </c>
       <c r="C52">
+        <f>'CEArun Nescius'!C62</f>
         <v>3226.98</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>237.12693222575854</v>
-      </c>
-      <c r="E52" s="15">
+        <v>230.18747641235291</v>
+      </c>
+      <c r="E52" s="13">
         <f t="shared" si="1"/>
-        <v>3.6450528869411852E-5</v>
+        <v>1.5977701785155975E-4</v>
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
         <v>3225.854442551019</v>
       </c>
-      <c r="G52" s="15">
+      <c r="G52" s="13">
         <f t="shared" si="3"/>
         <v>3.4879591722942154E-4</v>
       </c>
@@ -31061,25 +31111,26 @@
         <v>3.0499999999999976</v>
       </c>
       <c r="B53">
-        <f>'CEArun Nescius'!D54</f>
-        <v>236.3302752293578</v>
+        <f>'CEArun Nescius'!D63</f>
+        <v>229.50050968399592</v>
       </c>
       <c r="C53">
+        <f>'CEArun Nescius'!C63</f>
         <v>3218.61</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
-        <v>236.26095084075951</v>
-      </c>
-      <c r="E53" s="15">
+        <v>229.49368629721516</v>
+      </c>
+      <c r="E53" s="13">
         <f t="shared" si="1"/>
-        <v>2.9333689274897338E-4</v>
+        <v>2.9731466784746497E-5</v>
       </c>
       <c r="F53">
         <f t="shared" si="2"/>
         <v>3218.1714483753749</v>
       </c>
-      <c r="G53" s="15">
+      <c r="G53" s="13">
         <f t="shared" si="3"/>
         <v>1.3625497485723144E-4</v>
       </c>
@@ -31089,25 +31140,26 @@
         <v>3.0999999999999974</v>
       </c>
       <c r="B54">
-        <f>'CEArun Nescius'!D55</f>
-        <v>235.53516819571863</v>
+        <f>'CEArun Nescius'!D64</f>
+        <v>228.78695208970439</v>
       </c>
       <c r="C54">
+        <f>'CEArun Nescius'!C64</f>
         <v>3210.14</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
-        <v>235.4164812164463</v>
-      </c>
-      <c r="E54" s="15">
+        <v>228.81506704291314</v>
+      </c>
+      <c r="E54" s="13">
         <f t="shared" si="1"/>
-        <v>5.0390343056414596E-4</v>
+        <v>1.2288704819903051E-4</v>
       </c>
       <c r="F54">
         <f t="shared" si="2"/>
         <v>3210.618330826037</v>
       </c>
-      <c r="G54" s="15">
+      <c r="G54" s="13">
         <f t="shared" si="3"/>
         <v>1.4900621967799181E-4</v>
       </c>
@@ -31117,25 +31169,26 @@
         <v>3.1499999999999972</v>
       </c>
       <c r="B55">
-        <f>'CEArun Nescius'!D56</f>
-        <v>234.75025484199796</v>
+        <f>'CEArun Nescius'!D65</f>
+        <v>228.08358817533127</v>
       </c>
       <c r="C55">
+        <f>'CEArun Nescius'!C65</f>
         <v>3201.58</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>234.6101822929968</v>
-      </c>
-      <c r="E55" s="15">
+        <v>228.14080978656443</v>
+      </c>
+      <c r="E55" s="13">
         <f t="shared" si="1"/>
-        <v>5.9668752690146727E-4</v>
+        <v>2.5088000276974405E-4</v>
       </c>
       <c r="F55">
         <f t="shared" si="2"/>
         <v>3202.9436305955023</v>
       </c>
-      <c r="G55" s="15">
+      <c r="G55" s="13">
         <f t="shared" si="3"/>
         <v>4.2592426099063589E-4</v>
       </c>
@@ -31145,25 +31198,26 @@
         <v>3.1999999999999971</v>
       </c>
       <c r="B56">
-        <f>'CEArun Nescius'!D57</f>
-        <v>233.97553516819573</v>
+        <f>'CEArun Nescius'!D66</f>
+        <v>227.38022426095819</v>
       </c>
       <c r="C56">
+        <f>'CEArun Nescius'!C66</f>
         <v>3192.92</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>233.86129909567626</v>
-      </c>
-      <c r="E56" s="15">
+        <v>227.45316181489807</v>
+      </c>
+      <c r="E56" s="13">
         <f t="shared" si="1"/>
-        <v>4.8823938980353262E-4</v>
+        <v>3.2077351571336188E-4</v>
       </c>
       <c r="F56">
         <f t="shared" si="2"/>
         <v>3194.7019792286592</v>
       </c>
-      <c r="G56" s="15">
+      <c r="G56" s="13">
         <f t="shared" si="3"/>
         <v>5.5810331253495571E-4</v>
       </c>
@@ -31173,25 +31227,26 @@
         <v>3.2499999999999969</v>
       </c>
       <c r="B57">
-        <f>'CEArun Nescius'!D58</f>
-        <v>233.21100917431193</v>
+        <f>'CEArun Nescius'!D67</f>
+        <v>226.68705402650357</v>
       </c>
       <c r="C57">
+        <f>'CEArun Nescius'!C67</f>
         <v>3184.18</v>
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
-        <v>233.19089128634096</v>
-      </c>
-      <c r="E57" s="15">
+        <v>226.7255790418626</v>
+      </c>
+      <c r="E57" s="13">
         <f t="shared" si="1"/>
-        <v>8.6264743856632092E-5</v>
+        <v>1.6994801721020874E-4</v>
       </c>
       <c r="F57">
         <f t="shared" si="2"/>
         <v>3185.1984030323365</v>
       </c>
-      <c r="G57" s="15">
+      <c r="G57" s="13">
         <f t="shared" si="3"/>
         <v>3.1983211763677438E-4</v>
       </c>
@@ -31201,41 +31256,42 @@
         <v>3.2999999999999967</v>
       </c>
       <c r="B58">
-        <f>'CEArun Nescius'!D59</f>
-        <v>232.44648318042815</v>
+        <f>'CEArun Nescius'!D68</f>
+        <v>226.00407747196735</v>
       </c>
       <c r="C58">
+        <f>'CEArun Nescius'!C68</f>
         <v>3175.36</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>232.62076124674877</v>
-      </c>
-      <c r="E58" s="15">
+        <v>225.92063913027482</v>
+      </c>
+      <c r="E58" s="13">
         <f t="shared" si="1"/>
-        <v>7.4975565960852877E-4</v>
+        <v>3.691895412943472E-4</v>
       </c>
       <c r="F58">
         <f t="shared" si="2"/>
         <v>3173.4248225992924</v>
       </c>
-      <c r="G58" s="15">
+      <c r="G58" s="13">
         <f t="shared" si="3"/>
         <v>6.0943559177785943E-4</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="16">
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="14">
         <f>MEDIAN(E2:E58)</f>
-        <v>6.9802317649149035E-4</v>
-      </c>
-      <c r="G59" s="16">
+        <v>2.409731563302448E-4</v>
+      </c>
+      <c r="G59" s="14">
         <f>MEDIAN(G2:G58)</f>
         <v>4.5338772384444416E-4</v>
       </c>

</xml_diff>